<commit_message>
causal_10k_scen3_sim_summ_tib re-run of 1000 point0/Hevo causal fixed
</commit_message>
<xml_diff>
--- a/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/Citations_Instrument_Data.xlsx
+++ b/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/Citations_Instrument_Data.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f99f7067dc2a9a5/Documents/R/Working Directory/Data_Science_MSc/Dissertation_Bayes_MR/MSc_Thesis/MSc_Thesis_Split/Data/Citations_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{D0FD9711-2C99-4E6F-B2AE-5B7E42B34EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5632B23-BA67-4A45-8825-DAAAD969CD32}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{D0FD9711-2C99-4E6F-B2AE-5B7E42B34EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11166E3D-78F7-488B-AEDD-AAAEF512F1C6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{CC9CB5CD-CE5C-4279-A491-567F2CB78E4D}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{CC9CB5CD-CE5C-4279-A491-567F2CB78E4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Citations_Instrument_Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12554" uniqueCount="2135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13188" uniqueCount="2247">
   <si>
     <t>Study_Ref</t>
   </si>
@@ -6425,16 +6438,353 @@
   </si>
   <si>
     <t>rs11090631</t>
+  </si>
+  <si>
+    <t>[@xu_causal_2022]</t>
+  </si>
+  <si>
+    <t>10.3389/fimmu.2021.746998</t>
+  </si>
+  <si>
+    <t>Coeliac Disease</t>
+  </si>
+  <si>
+    <t>Gut Bifidobacterium</t>
+  </si>
+  <si>
+    <t>rs1018326</t>
+  </si>
+  <si>
+    <t>rs10456362</t>
+  </si>
+  <si>
+    <t>rs10498722</t>
+  </si>
+  <si>
+    <t>rs1050976</t>
+  </si>
+  <si>
+    <t>rs10513548</t>
+  </si>
+  <si>
+    <t>rs10800746</t>
+  </si>
+  <si>
+    <t>rs10892258</t>
+  </si>
+  <si>
+    <t>rs10946938</t>
+  </si>
+  <si>
+    <t>rs11066320</t>
+  </si>
+  <si>
+    <t>rs1107943</t>
+  </si>
+  <si>
+    <t>rs11158</t>
+  </si>
+  <si>
+    <t>rs11801183</t>
+  </si>
+  <si>
+    <t>rs11851414</t>
+  </si>
+  <si>
+    <t>rs11875687</t>
+  </si>
+  <si>
+    <t>rs12068671</t>
+  </si>
+  <si>
+    <t>rs1233405</t>
+  </si>
+  <si>
+    <t>rs1250552</t>
+  </si>
+  <si>
+    <t>rs13003464</t>
+  </si>
+  <si>
+    <t>rs1311918</t>
+  </si>
+  <si>
+    <t>rs13132308</t>
+  </si>
+  <si>
+    <t>rs13151961</t>
+  </si>
+  <si>
+    <t>rs13198474</t>
+  </si>
+  <si>
+    <t>rs13203715</t>
+  </si>
+  <si>
+    <t>rs13215054</t>
+  </si>
+  <si>
+    <t>rs13219354</t>
+  </si>
+  <si>
+    <t>rs1323292</t>
+  </si>
+  <si>
+    <t>rs1378938</t>
+  </si>
+  <si>
+    <t>rs1405490</t>
+  </si>
+  <si>
+    <t>rs149901</t>
+  </si>
+  <si>
+    <t>rs16891725</t>
+  </si>
+  <si>
+    <t>rs17264332</t>
+  </si>
+  <si>
+    <t>rs17475879</t>
+  </si>
+  <si>
+    <t>rs17630235</t>
+  </si>
+  <si>
+    <t>rs17693963</t>
+  </si>
+  <si>
+    <t>rs182429</t>
+  </si>
+  <si>
+    <t>rs1893592</t>
+  </si>
+  <si>
+    <t>rs1929848</t>
+  </si>
+  <si>
+    <t>rs1980422</t>
+  </si>
+  <si>
+    <t>rs2030519</t>
+  </si>
+  <si>
+    <t>rs209139</t>
+  </si>
+  <si>
+    <t>rs2097282</t>
+  </si>
+  <si>
+    <t>rs210196</t>
+  </si>
+  <si>
+    <t>rs2269426</t>
+  </si>
+  <si>
+    <t>rs2281820</t>
+  </si>
+  <si>
+    <t>rs2294478</t>
+  </si>
+  <si>
+    <t>rs2394401</t>
+  </si>
+  <si>
+    <t>rs2395309</t>
+  </si>
+  <si>
+    <t>rs241439</t>
+  </si>
+  <si>
+    <t>rs2499714</t>
+  </si>
+  <si>
+    <t>rs2517425</t>
+  </si>
+  <si>
+    <t>rs2517582</t>
+  </si>
+  <si>
+    <t>rs2524005</t>
+  </si>
+  <si>
+    <t>rs2736171</t>
+  </si>
+  <si>
+    <t>rs29218</t>
+  </si>
+  <si>
+    <t>rs3094228</t>
+  </si>
+  <si>
+    <t>rs3101942</t>
+  </si>
+  <si>
+    <t>rs3117143</t>
+  </si>
+  <si>
+    <t>rs3117324</t>
+  </si>
+  <si>
+    <t>rs3130531</t>
+  </si>
+  <si>
+    <t>rs3130934</t>
+  </si>
+  <si>
+    <t>rs3131622</t>
+  </si>
+  <si>
+    <t>rs3132584</t>
+  </si>
+  <si>
+    <t>rs3132645</t>
+  </si>
+  <si>
+    <t>rs3134942</t>
+  </si>
+  <si>
+    <t>rs3184504</t>
+  </si>
+  <si>
+    <t>rs34018127</t>
+  </si>
+  <si>
+    <t>rs3734840</t>
+  </si>
+  <si>
+    <t>rs3857546</t>
+  </si>
+  <si>
+    <t>rs3869145</t>
+  </si>
+  <si>
+    <t>rs4084096</t>
+  </si>
+  <si>
+    <t>rs4445406</t>
+  </si>
+  <si>
+    <t>rs445870</t>
+  </si>
+  <si>
+    <t>rs4713646</t>
+  </si>
+  <si>
+    <t>rs4821124</t>
+  </si>
+  <si>
+    <t>rs4947256</t>
+  </si>
+  <si>
+    <t>rs4947324</t>
+  </si>
+  <si>
+    <t>rs525623</t>
+  </si>
+  <si>
+    <t>rs55743914</t>
+  </si>
+  <si>
+    <t>rs61579022</t>
+  </si>
+  <si>
+    <t>rs61907765</t>
+  </si>
+  <si>
+    <t>rs6498114</t>
+  </si>
+  <si>
+    <t>rs652888</t>
+  </si>
+  <si>
+    <t>rs6715106</t>
+  </si>
+  <si>
+    <t>rs6904165</t>
+  </si>
+  <si>
+    <t>rs6921948</t>
+  </si>
+  <si>
+    <t>rs6930435</t>
+  </si>
+  <si>
+    <t>rs6941621</t>
+  </si>
+  <si>
+    <t>rs7104791</t>
+  </si>
+  <si>
+    <t>rs742132</t>
+  </si>
+  <si>
+    <t>rs744254</t>
+  </si>
+  <si>
+    <t>rs7616215</t>
+  </si>
+  <si>
+    <t>rs762324</t>
+  </si>
+  <si>
+    <t>rs76830965</t>
+  </si>
+  <si>
+    <t>rs7749305</t>
+  </si>
+  <si>
+    <t>rs78000963</t>
+  </si>
+  <si>
+    <t>rs79758729</t>
+  </si>
+  <si>
+    <t>rs806977</t>
+  </si>
+  <si>
+    <t>rs9261564</t>
+  </si>
+  <si>
+    <t>rs9268326</t>
+  </si>
+  <si>
+    <t>rs9268877</t>
+  </si>
+  <si>
+    <t>rs9272219</t>
+  </si>
+  <si>
+    <t>rs9275224</t>
+  </si>
+  <si>
+    <t>rs9295661</t>
+  </si>
+  <si>
+    <t>rs9404942</t>
+  </si>
+  <si>
+    <t>rs990171</t>
+  </si>
+  <si>
+    <t>[@budu-aggrey_evidence_2019]</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pmed.1002739</t>
+  </si>
+  <si>
+    <t>Psoriasis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6574,6 +6924,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -6757,7 +7113,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -6872,6 +7228,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -6917,9 +7282,27 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6976,6 +7359,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7295,13 +7682,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7656F3E6-3E4C-4A5B-B3D8-43D3B6FC3335}">
-  <dimension ref="A1:J2081"/>
+  <dimension ref="A1:J2186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2078" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2081" sqref="A2081"/>
+      <selection pane="bottomRight" activeCell="F2186" sqref="F2186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -73876,7 +74263,3380 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="2081" collapsed="1" x14ac:dyDescent="0.35"/>
+    <row r="2081" spans="1:10" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A2081" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2081" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2081" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2081" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2081" s="2" t="s">
+        <v>2139</v>
+      </c>
+      <c r="F2081" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2081" s="4">
+        <v>0.151862349309246</v>
+      </c>
+      <c r="H2081" s="4">
+        <v>1.85859371207363E-2</v>
+      </c>
+      <c r="I2081" s="6">
+        <v>-1.231266E-3</v>
+      </c>
+      <c r="J2081" s="4">
+        <v>1.1824049999999999E-2</v>
+      </c>
+    </row>
+    <row r="2082" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2082" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2082" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2082" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2082" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2082" s="2" t="s">
+        <v>2140</v>
+      </c>
+      <c r="F2082" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2082" s="4">
+        <v>0.85271175023128398</v>
+      </c>
+      <c r="H2082" s="4">
+        <v>2.4574517232816201E-2</v>
+      </c>
+      <c r="I2082" s="4">
+        <v>5.9405079999999997E-3</v>
+      </c>
+      <c r="J2082" s="4">
+        <v>1.6688209999999998E-2</v>
+      </c>
+    </row>
+    <row r="2083" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2083" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2083" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2083" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2083" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2083" s="2" t="s">
+        <v>2141</v>
+      </c>
+      <c r="F2083" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2083" s="4">
+        <v>0.50802169643325601</v>
+      </c>
+      <c r="H2083" s="4">
+        <v>3.0682549433893501E-2</v>
+      </c>
+      <c r="I2083" s="4">
+        <v>-1.2598959999999999E-2</v>
+      </c>
+      <c r="J2083" s="4">
+        <v>2.136747E-2</v>
+      </c>
+    </row>
+    <row r="2084" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2084" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2084" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2084" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2084" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2084" s="2" t="s">
+        <v>2142</v>
+      </c>
+      <c r="F2084" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2084" s="4">
+        <v>-0.111043298793325</v>
+      </c>
+      <c r="H2084" s="4">
+        <v>1.8471772837446301E-2</v>
+      </c>
+      <c r="I2084" s="4">
+        <v>-9.6217739999999996E-3</v>
+      </c>
+      <c r="J2084" s="4">
+        <v>1.174775E-2</v>
+      </c>
+    </row>
+    <row r="2085" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2085" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2085" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2085" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2085" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2085" s="2" t="s">
+        <v>2143</v>
+      </c>
+      <c r="F2085" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2085" s="4">
+        <v>-0.185847766570513</v>
+      </c>
+      <c r="H2085" s="4">
+        <v>3.3908857972428201E-2</v>
+      </c>
+      <c r="I2085" s="6">
+        <v>-3.9026579999999998E-3</v>
+      </c>
+      <c r="J2085" s="4">
+        <v>2.071771E-2</v>
+      </c>
+    </row>
+    <row r="2086" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2086" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2086" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2086" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2086" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2086" s="2" t="s">
+        <v>2144</v>
+      </c>
+      <c r="F2086" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2086" s="4">
+        <v>-0.11216136688833001</v>
+      </c>
+      <c r="H2086" s="4">
+        <v>2.0142258104921901E-2</v>
+      </c>
+      <c r="I2086" s="4">
+        <v>-3.24384067027031E-2</v>
+      </c>
+      <c r="J2086" s="4">
+        <v>1.27589640795379E-2</v>
+      </c>
+    </row>
+    <row r="2087" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2087" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2087" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2087" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2087" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2087" s="2" t="s">
+        <v>2145</v>
+      </c>
+      <c r="F2087" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2087" s="4">
+        <v>-0.14954463728001799</v>
+      </c>
+      <c r="H2087" s="4">
+        <v>2.2231073718118499E-2</v>
+      </c>
+      <c r="I2087" s="4">
+        <v>-1.5572095054369199E-2</v>
+      </c>
+      <c r="J2087" s="4">
+        <v>1.38969808758729E-2</v>
+      </c>
+    </row>
+    <row r="2088" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2088" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2088" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2088" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2088" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2088" s="2" t="s">
+        <v>2146</v>
+      </c>
+      <c r="F2088" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2088" s="4">
+        <v>-0.211585602480481</v>
+      </c>
+      <c r="H2088" s="4">
+        <v>2.2462099102081301E-2</v>
+      </c>
+      <c r="I2088" s="4">
+        <v>1.3737350000000001E-2</v>
+      </c>
+      <c r="J2088" s="4">
+        <v>1.340909E-2</v>
+      </c>
+    </row>
+    <row r="2089" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2089" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2089" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2089" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2089" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2089" s="2" t="s">
+        <v>2147</v>
+      </c>
+      <c r="F2089" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2089" s="4">
+        <v>0.13889199886661899</v>
+      </c>
+      <c r="H2089" s="4">
+        <v>1.8711915818992599E-2</v>
+      </c>
+      <c r="I2089" s="4">
+        <v>1.2337748669226699E-2</v>
+      </c>
+      <c r="J2089" s="4">
+        <v>1.1983564035795599E-2</v>
+      </c>
+    </row>
+    <row r="2090" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2090" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2090" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2090" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2090" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2090" s="2" t="s">
+        <v>2148</v>
+      </c>
+      <c r="F2090" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2090" s="4">
+        <v>0.19967019512856801</v>
+      </c>
+      <c r="H2090" s="4">
+        <v>3.4607541108987103E-2</v>
+      </c>
+      <c r="I2090" s="4">
+        <v>-1.4964999999999999E-2</v>
+      </c>
+      <c r="J2090" s="4">
+        <v>2.305668E-2</v>
+      </c>
+    </row>
+    <row r="2091" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2091" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2091" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2091" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2091" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2091" s="2" t="s">
+        <v>2149</v>
+      </c>
+      <c r="F2091" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2091" s="4">
+        <v>1.39624469197306</v>
+      </c>
+      <c r="H2091" s="4">
+        <v>3.6296825054164102E-2</v>
+      </c>
+      <c r="I2091" s="4">
+        <v>5.6600610000000001E-3</v>
+      </c>
+      <c r="J2091" s="4">
+        <v>2.2437450000000001E-2</v>
+      </c>
+    </row>
+    <row r="2092" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2092" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2092" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2092" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2092" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2092" s="2" t="s">
+        <v>2150</v>
+      </c>
+      <c r="F2092" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2092" s="4">
+        <v>-0.13834294962174501</v>
+      </c>
+      <c r="H2092" s="4">
+        <v>2.4522924358550701E-2</v>
+      </c>
+      <c r="I2092" s="4">
+        <v>-2.5389191534332299E-2</v>
+      </c>
+      <c r="J2092" s="4">
+        <v>1.54001886287748E-2</v>
+      </c>
+    </row>
+    <row r="2093" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2093" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2093" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2093" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2093" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2093" s="2" t="s">
+        <v>2151</v>
+      </c>
+      <c r="F2093" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2093" s="4">
+        <v>0.12044615307586699</v>
+      </c>
+      <c r="H2093" s="4">
+        <v>2.2051200627930399E-2</v>
+      </c>
+      <c r="I2093" s="4">
+        <v>-1.69064514653594E-2</v>
+      </c>
+      <c r="J2093" s="4">
+        <v>1.43138393702976E-2</v>
+      </c>
+    </row>
+    <row r="2094" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2094" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2094" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2094" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2094" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2094" s="2" t="s">
+        <v>2152</v>
+      </c>
+      <c r="F2094" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2094" s="4">
+        <v>0.159564569671338</v>
+      </c>
+      <c r="H2094" s="4">
+        <v>2.5057852322354902E-2</v>
+      </c>
+      <c r="I2094" s="4">
+        <v>1.49313E-2</v>
+      </c>
+      <c r="J2094" s="4">
+        <v>1.5337190000000001E-2</v>
+      </c>
+    </row>
+    <row r="2095" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2095" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2095" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2095" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2095" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2095" s="2" t="s">
+        <v>2153</v>
+      </c>
+      <c r="F2095" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2095" s="4">
+        <v>-0.15665381004537701</v>
+      </c>
+      <c r="H2095" s="4">
+        <v>2.4415282307669699E-2</v>
+      </c>
+      <c r="I2095" s="4">
+        <v>7.741052E-3</v>
+      </c>
+      <c r="J2095" s="4">
+        <v>1.554065E-2</v>
+      </c>
+    </row>
+    <row r="2096" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2096" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2096" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2096" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2096" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2096" s="2" t="s">
+        <v>2154</v>
+      </c>
+      <c r="F2096" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2096" s="4">
+        <v>-0.384486701722973</v>
+      </c>
+      <c r="H2096" s="4">
+        <v>1.9052010116400699E-2</v>
+      </c>
+      <c r="I2096" s="6">
+        <v>7.8783520000000004E-4</v>
+      </c>
+      <c r="J2096" s="4">
+        <v>1.18548E-2</v>
+      </c>
+    </row>
+    <row r="2097" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2097" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2097" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2097" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2097" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2097" s="2" t="s">
+        <v>2155</v>
+      </c>
+      <c r="F2097" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2097" s="4">
+        <v>-0.15478421380086599</v>
+      </c>
+      <c r="H2097" s="4">
+        <v>1.85777479752634E-2</v>
+      </c>
+      <c r="I2097" s="4">
+        <v>1.012682E-2</v>
+      </c>
+      <c r="J2097" s="4">
+        <v>1.170732E-2</v>
+      </c>
+    </row>
+    <row r="2098" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2098" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2098" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2098" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2098" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2098" s="2" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F2098" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2098" s="4">
+        <v>0.15357908792830099</v>
+      </c>
+      <c r="H2098" s="4">
+        <v>1.8893425648131401E-2</v>
+      </c>
+      <c r="I2098" s="4">
+        <v>7.427988E-3</v>
+      </c>
+      <c r="J2098" s="4">
+        <v>1.222786E-2</v>
+      </c>
+    </row>
+    <row r="2099" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2099" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2099" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2099" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2099" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2099" s="2" t="s">
+        <v>2157</v>
+      </c>
+      <c r="F2099" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2099" s="4">
+        <v>1.2345989978677001</v>
+      </c>
+      <c r="H2099" s="4">
+        <v>3.2094678028337202E-2</v>
+      </c>
+      <c r="I2099" s="4">
+        <v>1.5821470000000001E-2</v>
+      </c>
+      <c r="J2099" s="4">
+        <v>2.1643550000000001E-2</v>
+      </c>
+    </row>
+    <row r="2100" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2100" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2100" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2100" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2100" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2100" s="2" t="s">
+        <v>2158</v>
+      </c>
+      <c r="F2100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2100" s="4">
+        <v>-0.348990261180185</v>
+      </c>
+      <c r="H2100" s="4">
+        <v>2.6913084488210701E-2</v>
+      </c>
+      <c r="I2100" s="4">
+        <v>-2.5774955106394999E-2</v>
+      </c>
+      <c r="J2100" s="4">
+        <v>1.6627455063032998E-2</v>
+      </c>
+    </row>
+    <row r="2101" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2101" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2101" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2101" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2101" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2101" s="2" t="s">
+        <v>2159</v>
+      </c>
+      <c r="F2101" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2101" s="4">
+        <v>-0.33547273628812901</v>
+      </c>
+      <c r="H2101" s="4">
+        <v>2.67872710488057E-2</v>
+      </c>
+      <c r="I2101" s="4">
+        <v>-2.0769639999999999E-2</v>
+      </c>
+      <c r="J2101" s="4">
+        <v>1.6645409999999999E-2</v>
+      </c>
+    </row>
+    <row r="2102" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2102" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2102" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2102" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2102" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2102" s="2" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F2102" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2102" s="4">
+        <v>0.94623780824210701</v>
+      </c>
+      <c r="H2102" s="4">
+        <v>3.1183146179035399E-2</v>
+      </c>
+      <c r="I2102" s="6">
+        <v>-2.7210730000000001E-3</v>
+      </c>
+      <c r="J2102" s="4">
+        <v>2.3732010000000001E-2</v>
+      </c>
+    </row>
+    <row r="2103" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2103" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2103" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2103" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2103" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2103" s="2" t="s">
+        <v>2161</v>
+      </c>
+      <c r="F2103" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2103" s="4">
+        <v>-0.36168748576227699</v>
+      </c>
+      <c r="H2103" s="4">
+        <v>3.0901075009991799E-2</v>
+      </c>
+      <c r="I2103" s="4">
+        <v>-1.0442140000000001E-2</v>
+      </c>
+      <c r="J2103" s="4">
+        <v>1.7425880000000001E-2</v>
+      </c>
+    </row>
+    <row r="2104" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2104" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2104" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2104" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2104" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2104" s="2" t="s">
+        <v>2162</v>
+      </c>
+      <c r="F2104" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2104" s="4">
+        <v>0.64605557302609495</v>
+      </c>
+      <c r="H2104" s="4">
+        <v>2.1115168646338701E-2</v>
+      </c>
+      <c r="I2104" s="4">
+        <v>8.1959900000000002E-3</v>
+      </c>
+      <c r="J2104" s="4">
+        <v>1.399195E-2</v>
+      </c>
+    </row>
+    <row r="2105" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2105" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2105" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2105" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2105" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2105" s="2" t="s">
+        <v>2163</v>
+      </c>
+      <c r="F2105" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2105" s="4">
+        <v>0.90138011913840099</v>
+      </c>
+      <c r="H2105" s="4">
+        <v>2.65050135254573E-2</v>
+      </c>
+      <c r="I2105" s="4">
+        <v>-1.153087E-2</v>
+      </c>
+      <c r="J2105" s="4">
+        <v>1.9060339999999999E-2</v>
+      </c>
+    </row>
+    <row r="2106" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2106" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2106" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2106" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2106" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2106" s="2" t="s">
+        <v>2164</v>
+      </c>
+      <c r="F2106" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2106" s="4">
+        <v>-0.26175445044186502</v>
+      </c>
+      <c r="H2106" s="4">
+        <v>2.5293016642340502E-2</v>
+      </c>
+      <c r="I2106" s="4">
+        <v>1.393231E-2</v>
+      </c>
+      <c r="J2106" s="4">
+        <v>1.498296E-2</v>
+      </c>
+    </row>
+    <row r="2107" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2107" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2107" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2107" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2107" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2107" s="2" t="s">
+        <v>2165</v>
+      </c>
+      <c r="F2107" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2107" s="4">
+        <v>0.117783035656383</v>
+      </c>
+      <c r="H2107" s="4">
+        <v>2.0402683646497399E-2</v>
+      </c>
+      <c r="I2107" s="6">
+        <v>-9.964199E-4</v>
+      </c>
+      <c r="J2107" s="4">
+        <v>1.284573E-2</v>
+      </c>
+    </row>
+    <row r="2108" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2108" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2108" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2108" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2108" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2108" s="2" t="s">
+        <v>2166</v>
+      </c>
+      <c r="F2108" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2108" s="4">
+        <v>0.11064652008706399</v>
+      </c>
+      <c r="H2108" s="4">
+        <v>2.0149119758920201E-2</v>
+      </c>
+      <c r="I2108" s="6">
+        <v>-3.1591829999999999E-3</v>
+      </c>
+      <c r="J2108" s="4">
+        <v>1.2619979999999999E-2</v>
+      </c>
+    </row>
+    <row r="2109" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2109" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2109" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2109" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2109" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2109" s="2" t="s">
+        <v>2167</v>
+      </c>
+      <c r="F2109" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2109" s="4">
+        <v>0.64710324205853798</v>
+      </c>
+      <c r="H2109" s="4">
+        <v>2.1224626321718301E-2</v>
+      </c>
+      <c r="I2109" s="4">
+        <v>2.2350288653683999E-2</v>
+      </c>
+      <c r="J2109" s="4">
+        <v>1.3662403659404101E-2</v>
+      </c>
+    </row>
+    <row r="2110" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2110" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2110" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2110" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2110" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2110" s="2" t="s">
+        <v>2168</v>
+      </c>
+      <c r="F2110" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2110" s="4">
+        <v>0.89527136465007995</v>
+      </c>
+      <c r="H2110" s="4">
+        <v>2.63005942673274E-2</v>
+      </c>
+      <c r="I2110" s="6">
+        <v>-2.0094959999999999E-3</v>
+      </c>
+      <c r="J2110" s="4">
+        <v>1.834212E-2</v>
+      </c>
+    </row>
+    <row r="2111" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2111" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2111" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2111" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2111" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2111" s="2" t="s">
+        <v>2169</v>
+      </c>
+      <c r="F2111" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2111" s="4">
+        <v>0.250758718347183</v>
+      </c>
+      <c r="H2111" s="4">
+        <v>2.2025907887938002E-2</v>
+      </c>
+      <c r="I2111" s="4">
+        <v>1.121893E-2</v>
+      </c>
+      <c r="J2111" s="4">
+        <v>1.5110439999999999E-2</v>
+      </c>
+    </row>
+    <row r="2112" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2112" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2112" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2112" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2112" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2112" s="2" t="s">
+        <v>2170</v>
+      </c>
+      <c r="F2112" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2112" s="4">
+        <v>-0.41354768430152</v>
+      </c>
+      <c r="H2112" s="4">
+        <v>4.0333227484368302E-2</v>
+      </c>
+      <c r="I2112" s="4">
+        <v>2.14437E-2</v>
+      </c>
+      <c r="J2112" s="4">
+        <v>2.7166829999999999E-2</v>
+      </c>
+    </row>
+    <row r="2113" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2113" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2113" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2113" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2113" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2113" s="2" t="s">
+        <v>2171</v>
+      </c>
+      <c r="F2113" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2113" s="4">
+        <v>0.151862349309246</v>
+      </c>
+      <c r="H2113" s="4">
+        <v>1.8756627704762E-2</v>
+      </c>
+      <c r="I2113" s="4">
+        <v>7.8806450000000004E-3</v>
+      </c>
+      <c r="J2113" s="4">
+        <v>1.203768E-2</v>
+      </c>
+    </row>
+    <row r="2114" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2114" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2114" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2114" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2114" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2114" s="2" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F2114" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2114" s="4">
+        <v>1.08316018410919</v>
+      </c>
+      <c r="H2114" s="4">
+        <v>2.8157869415202801E-2</v>
+      </c>
+      <c r="I2114" s="6">
+        <v>4.0335570000000001E-3</v>
+      </c>
+      <c r="J2114" s="4">
+        <v>2.110687E-2</v>
+      </c>
+    </row>
+    <row r="2115" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2115" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2115" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2115" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2115" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2115" s="2" t="s">
+        <v>2173</v>
+      </c>
+      <c r="F2115" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2115" s="4">
+        <v>0.15014265842971899</v>
+      </c>
+      <c r="H2115" s="4">
+        <v>1.8658254826382802E-2</v>
+      </c>
+      <c r="I2115" s="4">
+        <v>-5.0974640000000003E-3</v>
+      </c>
+      <c r="J2115" s="4">
+        <v>1.1817619999999999E-2</v>
+      </c>
+    </row>
+    <row r="2116" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2116" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2116" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2116" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2116" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2116" s="2" t="s">
+        <v>2174</v>
+      </c>
+      <c r="F2116" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2116" s="4">
+        <v>-0.12386398722238599</v>
+      </c>
+      <c r="H2116" s="4">
+        <v>2.08748912747347E-2</v>
+      </c>
+      <c r="I2116" s="4">
+        <v>1.2604219999999999E-2</v>
+      </c>
+      <c r="J2116" s="4">
+        <v>1.3028619999999999E-2</v>
+      </c>
+    </row>
+    <row r="2117" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2117" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2117" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2117" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2117" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2117" s="2" t="s">
+        <v>2175</v>
+      </c>
+      <c r="F2117" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2117" s="4">
+        <v>0.188966099512623</v>
+      </c>
+      <c r="H2117" s="4">
+        <v>2.6164008853986401E-2</v>
+      </c>
+      <c r="I2117" s="4">
+        <v>3.57224638748646E-2</v>
+      </c>
+      <c r="J2117" s="4">
+        <v>1.7481800170896102E-2</v>
+      </c>
+    </row>
+    <row r="2118" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2118" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2118" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2118" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2118" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2118" s="2" t="s">
+        <v>2176</v>
+      </c>
+      <c r="F2118" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2118" s="4">
+        <v>0.172271220940453</v>
+      </c>
+      <c r="H2118" s="4">
+        <v>2.1579481803826399E-2</v>
+      </c>
+      <c r="I2118" s="4">
+        <v>-2.1694885227548099E-2</v>
+      </c>
+      <c r="J2118" s="4">
+        <v>1.4051232300383701E-2</v>
+      </c>
+    </row>
+    <row r="2119" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2119" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2119" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2119" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2119" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2119" s="2" t="s">
+        <v>2177</v>
+      </c>
+      <c r="F2119" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2119" s="4">
+        <v>-0.27825993387287601</v>
+      </c>
+      <c r="H2119" s="4">
+        <v>1.8862903001002299E-2</v>
+      </c>
+      <c r="I2119" s="4">
+        <v>-6.7746589999999997E-3</v>
+      </c>
+      <c r="J2119" s="4">
+        <v>1.171261E-2</v>
+      </c>
+    </row>
+    <row r="2120" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2120" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2120" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2120" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2120" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2120" s="2" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F2120" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2120" s="4">
+        <v>-0.297328449503586</v>
+      </c>
+      <c r="H2120" s="4">
+        <v>4.19656453824412E-2</v>
+      </c>
+      <c r="I2120" s="6">
+        <v>-3.5708760000000002E-3</v>
+      </c>
+      <c r="J2120" s="4">
+        <v>2.9832839999999999E-2</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2121" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2121" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2121" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2121" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2121" s="2" t="s">
+        <v>2179</v>
+      </c>
+      <c r="F2121" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2121" s="4">
+        <v>0.183986836113016</v>
+      </c>
+      <c r="H2121" s="4">
+        <v>1.9734533079407701E-2</v>
+      </c>
+      <c r="I2121" s="4">
+        <v>-5.2036570000000004E-3</v>
+      </c>
+      <c r="J2121" s="4">
+        <v>1.253814E-2</v>
+      </c>
+    </row>
+    <row r="2122" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2122" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2122" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2122" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2122" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2122" s="2" t="s">
+        <v>2180</v>
+      </c>
+      <c r="F2122" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2122" s="4">
+        <v>-0.18548656013711101</v>
+      </c>
+      <c r="H2122" s="4">
+        <v>2.0196896111315699E-2</v>
+      </c>
+      <c r="I2122" s="4">
+        <v>2.6490871987481599E-2</v>
+      </c>
+      <c r="J2122" s="4">
+        <v>1.30491765621674E-2</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2123" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2123" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2123" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2123" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2123" s="2" t="s">
+        <v>2181</v>
+      </c>
+      <c r="F2123" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2123" s="4">
+        <v>-0.76894889397622701</v>
+      </c>
+      <c r="H2123" s="4">
+        <v>2.14254096157524E-2</v>
+      </c>
+      <c r="I2123" s="4">
+        <v>3.65483386413199E-2</v>
+      </c>
+      <c r="J2123" s="4">
+        <v>1.2038360391307601E-2</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2124" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2124" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2124" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2124" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2124" s="2" t="s">
+        <v>2182</v>
+      </c>
+      <c r="F2124" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2124" s="4">
+        <v>0.28743204119657201</v>
+      </c>
+      <c r="H2124" s="4">
+        <v>1.8839085964213902E-2</v>
+      </c>
+      <c r="I2124" s="4">
+        <v>-1.84183304667172E-2</v>
+      </c>
+      <c r="J2124" s="4">
+        <v>1.1892584372819299E-2</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2125" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2125" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2125" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2125" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2125" s="2" t="s">
+        <v>2183</v>
+      </c>
+      <c r="F2125" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2125" s="4">
+        <v>-0.45870766950388397</v>
+      </c>
+      <c r="H2125" s="4">
+        <v>1.9185142187911002E-2</v>
+      </c>
+      <c r="I2125" s="4">
+        <v>1.50762179609671E-2</v>
+      </c>
+      <c r="J2125" s="4">
+        <v>1.18679293898172E-2</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2126" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2126" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2126" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2126" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2126" s="2" t="s">
+        <v>2184</v>
+      </c>
+      <c r="F2126" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2126" s="4">
+        <v>-0.27918494219783502</v>
+      </c>
+      <c r="H2126" s="4">
+        <v>3.0901059094514498E-2</v>
+      </c>
+      <c r="I2126" s="4">
+        <v>1.7936919999999999E-2</v>
+      </c>
+      <c r="J2126" s="4">
+        <v>2.0271689999999998E-2</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2127" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2127" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2127" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2127" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2127" s="2" t="s">
+        <v>2185</v>
+      </c>
+      <c r="F2127" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2127" s="4">
+        <v>0.68662596356967998</v>
+      </c>
+      <c r="H2127" s="4">
+        <v>2.2173313094904099E-2</v>
+      </c>
+      <c r="I2127" s="4">
+        <v>7.0599269999999997E-3</v>
+      </c>
+      <c r="J2127" s="4">
+        <v>1.488576E-2</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2128" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2128" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2128" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2128" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2128" s="2" t="s">
+        <v>2186</v>
+      </c>
+      <c r="F2128" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2128" s="4">
+        <v>0.604862265692374</v>
+      </c>
+      <c r="H2128" s="4">
+        <v>1.9647323229975699E-2</v>
+      </c>
+      <c r="I2128" s="4">
+        <v>2.4489261997328898E-2</v>
+      </c>
+      <c r="J2128" s="4">
+        <v>1.19056538460229E-2</v>
+      </c>
+    </row>
+    <row r="2129" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2129" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2129" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2129" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2129" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2129" s="2" t="s">
+        <v>2187</v>
+      </c>
+      <c r="F2129" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2129" s="4">
+        <v>0.188966099512623</v>
+      </c>
+      <c r="H2129" s="4">
+        <v>3.0535304421552601E-2</v>
+      </c>
+      <c r="I2129" s="6">
+        <v>1.4181479999999999E-3</v>
+      </c>
+      <c r="J2129" s="4">
+        <v>1.8922660000000001E-2</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2130" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2130" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2130" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2130" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2130" s="2" t="s">
+        <v>2188</v>
+      </c>
+      <c r="F2130" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2130" s="4">
+        <v>0.83681453037235798</v>
+      </c>
+      <c r="H2130" s="4">
+        <v>2.17538593244615E-2</v>
+      </c>
+      <c r="I2130" s="4">
+        <v>8.9475100000000005E-3</v>
+      </c>
+      <c r="J2130" s="4">
+        <v>1.3370419999999999E-2</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2131" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2131" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2131" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2131" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2131" s="2" t="s">
+        <v>2189</v>
+      </c>
+      <c r="F2131" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2131" s="4">
+        <v>-0.63129977723386499</v>
+      </c>
+      <c r="H2131" s="4">
+        <v>2.0579327155416102E-2</v>
+      </c>
+      <c r="I2131" s="6">
+        <v>-1.7240129999999999E-3</v>
+      </c>
+      <c r="J2131" s="4">
+        <v>1.196083E-2</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2132" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2132" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2132" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2132" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2132" s="2" t="s">
+        <v>2190</v>
+      </c>
+      <c r="F2132" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2132" s="4">
+        <v>0.82767807351755096</v>
+      </c>
+      <c r="H2132" s="4">
+        <v>2.2502063069062099E-2</v>
+      </c>
+      <c r="I2132" s="4">
+        <v>1.196939E-2</v>
+      </c>
+      <c r="J2132" s="4">
+        <v>1.463922E-2</v>
+      </c>
+    </row>
+    <row r="2133" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2133" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2133" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2133" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2133" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2133" s="2" t="s">
+        <v>2191</v>
+      </c>
+      <c r="F2133" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2133" s="4">
+        <v>-1.0418539548495001</v>
+      </c>
+      <c r="H2133" s="4">
+        <v>2.7084071258113698E-2</v>
+      </c>
+      <c r="I2133" s="4">
+        <v>2.0770979691636899E-2</v>
+      </c>
+      <c r="J2133" s="4">
+        <v>1.1973270152404E-2</v>
+      </c>
+    </row>
+    <row r="2134" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2134" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2134" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2134" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2134" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2134" s="2" t="s">
+        <v>2192</v>
+      </c>
+      <c r="F2134" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2134" s="4">
+        <v>0.75565238591134198</v>
+      </c>
+      <c r="H2134" s="4">
+        <v>2.2217780487428E-2</v>
+      </c>
+      <c r="I2134" s="4">
+        <v>9.4913480000000001E-3</v>
+      </c>
+      <c r="J2134" s="4">
+        <v>1.409461E-2</v>
+      </c>
+    </row>
+    <row r="2135" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2135" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2135" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2135" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2135" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2135" s="2" t="s">
+        <v>2193</v>
+      </c>
+      <c r="F2135" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2135" s="4">
+        <v>1.4504421809436401</v>
+      </c>
+      <c r="H2135" s="4">
+        <v>3.7705744842256798E-2</v>
+      </c>
+      <c r="I2135" s="4">
+        <v>-2.3550185220780302E-2</v>
+      </c>
+      <c r="J2135" s="4">
+        <v>1.5401254852237201E-2</v>
+      </c>
+    </row>
+    <row r="2136" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2136" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2136" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2136" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2136" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2136" s="2" t="s">
+        <v>2194</v>
+      </c>
+      <c r="F2136" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2136" s="4">
+        <v>-0.65971240447370805</v>
+      </c>
+      <c r="H2136" s="4">
+        <v>2.0706975028304E-2</v>
+      </c>
+      <c r="I2136" s="4">
+        <v>1.49482321118497E-2</v>
+      </c>
+      <c r="J2136" s="4">
+        <v>1.19007182051377E-2</v>
+      </c>
+    </row>
+    <row r="2137" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2137" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2137" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2137" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2137" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2137" s="2" t="s">
+        <v>2195</v>
+      </c>
+      <c r="F2137" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2137" s="4">
+        <v>1.2501882281229</v>
+      </c>
+      <c r="H2137" s="4">
+        <v>3.2499936194441699E-2</v>
+      </c>
+      <c r="I2137" s="4">
+        <v>1.7026860000000001E-2</v>
+      </c>
+      <c r="J2137" s="4">
+        <v>2.1821699999999999E-2</v>
+      </c>
+    </row>
+    <row r="2138" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2138" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2138" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2138" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2138" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2138" s="2" t="s">
+        <v>2196</v>
+      </c>
+      <c r="F2138" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2138" s="4">
+        <v>0.30601302913650402</v>
+      </c>
+      <c r="H2138" s="4">
+        <v>1.8714098357952701E-2</v>
+      </c>
+      <c r="I2138" s="6">
+        <v>-1.1436980000000001E-3</v>
+      </c>
+      <c r="J2138" s="4">
+        <v>1.1894450000000001E-2</v>
+      </c>
+    </row>
+    <row r="2139" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2139" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2139" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2139" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2139" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2139" s="2" t="s">
+        <v>2197</v>
+      </c>
+      <c r="F2139" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2139" s="4">
+        <v>-0.54472717544167204</v>
+      </c>
+      <c r="H2139" s="4">
+        <v>2.0409293115960899E-2</v>
+      </c>
+      <c r="I2139" s="6">
+        <v>-3.3137129999999998E-3</v>
+      </c>
+      <c r="J2139" s="4">
+        <v>1.220182E-2</v>
+      </c>
+    </row>
+    <row r="2140" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2140" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2140" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2140" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2140" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2140" s="2" t="s">
+        <v>2198</v>
+      </c>
+      <c r="F2140" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2140" s="4">
+        <v>-0.70684050769194795</v>
+      </c>
+      <c r="H2140" s="4">
+        <v>2.24433844469176E-2</v>
+      </c>
+      <c r="I2140" s="6">
+        <v>1.3256489999999999E-3</v>
+      </c>
+      <c r="J2140" s="4">
+        <v>1.2272740000000001E-2</v>
+      </c>
+    </row>
+    <row r="2141" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2141" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2141" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2141" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2141" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2141" s="2" t="s">
+        <v>2199</v>
+      </c>
+      <c r="F2141" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2141" s="4">
+        <v>-0.63280495155378402</v>
+      </c>
+      <c r="H2141" s="4">
+        <v>1.9891426487262099E-2</v>
+      </c>
+      <c r="I2141" s="6">
+        <v>-3.061884E-3</v>
+      </c>
+      <c r="J2141" s="4">
+        <v>1.2065930000000001E-2</v>
+      </c>
+    </row>
+    <row r="2142" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2142" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2142" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2142" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2142" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2142" s="2" t="s">
+        <v>2200</v>
+      </c>
+      <c r="F2142" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2142" s="4">
+        <v>1.0553567799971499</v>
+      </c>
+      <c r="H2142" s="4">
+        <v>2.7435091165253798E-2</v>
+      </c>
+      <c r="I2142" s="6">
+        <v>7.9725809999999994E-3</v>
+      </c>
+      <c r="J2142" s="4">
+        <v>1.506948E-2</v>
+      </c>
+    </row>
+    <row r="2143" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2143" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2143" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2143" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2143" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2143" s="2" t="s">
+        <v>2201</v>
+      </c>
+      <c r="F2143" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2143" s="4">
+        <v>1.39624469197306</v>
+      </c>
+      <c r="H2143" s="4">
+        <v>3.6296825054164102E-2</v>
+      </c>
+      <c r="I2143" s="6">
+        <v>1.4890249999999999E-3</v>
+      </c>
+      <c r="J2143" s="4">
+        <v>2.196625E-2</v>
+      </c>
+    </row>
+    <row r="2144" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2144" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2144" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2144" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2144" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2144" s="2" t="s">
+        <v>2202</v>
+      </c>
+      <c r="F2144" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2144" s="4">
+        <v>1.92774617842764</v>
+      </c>
+      <c r="H2144" s="4">
+        <v>5.0113755983805498E-2</v>
+      </c>
+      <c r="I2144" s="4">
+        <v>-1.556252E-2</v>
+      </c>
+      <c r="J2144" s="4">
+        <v>1.77065E-2</v>
+      </c>
+    </row>
+    <row r="2145" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2145" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2145" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2145" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2145" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2145" s="2" t="s">
+        <v>2203</v>
+      </c>
+      <c r="F2145" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2145" s="4">
+        <v>0.17563256864315799</v>
+      </c>
+      <c r="H2145" s="4">
+        <v>1.8682881081075301E-2</v>
+      </c>
+      <c r="I2145" s="6">
+        <v>3.8197539999999999E-3</v>
+      </c>
+      <c r="J2145" s="4">
+        <v>1.183595E-2</v>
+      </c>
+    </row>
+    <row r="2146" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2146" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2146" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2146" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2146" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2146" s="2" t="s">
+        <v>2204</v>
+      </c>
+      <c r="F2146" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2146" s="4">
+        <v>-0.36701392173391201</v>
+      </c>
+      <c r="H2146" s="4">
+        <v>6.1774718188827599E-2</v>
+      </c>
+      <c r="I2146" s="4">
+        <v>-5.9290570000000001E-2</v>
+      </c>
+      <c r="J2146" s="4">
+        <v>5.4905580000000002E-2</v>
+      </c>
+    </row>
+    <row r="2147" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2147" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2147" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2147" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2147" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2147" s="2" t="s">
+        <v>2205</v>
+      </c>
+      <c r="F2147" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2147" s="4">
+        <v>-0.43417327224490798</v>
+      </c>
+      <c r="H2147" s="4">
+        <v>2.5432672070656099E-2</v>
+      </c>
+      <c r="I2147" s="4">
+        <v>-1.7146020000000001E-2</v>
+      </c>
+      <c r="J2147" s="4">
+        <v>1.6212799999999999E-2</v>
+      </c>
+    </row>
+    <row r="2148" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2148" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2148" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2148" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2148" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2148" s="2" t="s">
+        <v>2206</v>
+      </c>
+      <c r="F2148" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2148" s="4">
+        <v>0.77149614697092195</v>
+      </c>
+      <c r="H2148" s="4">
+        <v>2.5041766695563301E-2</v>
+      </c>
+      <c r="I2148" s="4">
+        <v>5.103036E-3</v>
+      </c>
+      <c r="J2148" s="4">
+        <v>1.8329149999999999E-2</v>
+      </c>
+    </row>
+    <row r="2149" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2149" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2149" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2149" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2149" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2149" s="2" t="s">
+        <v>2207</v>
+      </c>
+      <c r="F2149" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2149" s="4">
+        <v>-0.55477751129517305</v>
+      </c>
+      <c r="H2149" s="4">
+        <v>5.8767263560804202E-2</v>
+      </c>
+      <c r="I2149" s="4">
+        <v>-1.5114239999999999E-2</v>
+      </c>
+      <c r="J2149" s="4">
+        <v>5.1867990000000003E-2</v>
+      </c>
+    </row>
+    <row r="2150" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2150" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2150" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2150" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2150" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2150" s="2" t="s">
+        <v>2208</v>
+      </c>
+      <c r="F2150" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2150" s="4">
+        <v>-0.451456691959157</v>
+      </c>
+      <c r="H2150" s="4">
+        <v>2.8643787205827598E-2</v>
+      </c>
+      <c r="I2150" s="4">
+        <v>-1.892812E-2</v>
+      </c>
+      <c r="J2150" s="4">
+        <v>1.715299E-2</v>
+      </c>
+    </row>
+    <row r="2151" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2151" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2151" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2151" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2151" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2151" s="2" t="s">
+        <v>2209</v>
+      </c>
+      <c r="F2151" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2151" s="4">
+        <v>-0.136048844463276</v>
+      </c>
+      <c r="H2151" s="4">
+        <v>1.9734271434844401E-2</v>
+      </c>
+      <c r="I2151" s="6">
+        <v>-7.3792490000000003E-4</v>
+      </c>
+      <c r="J2151" s="4">
+        <v>1.226826E-2</v>
+      </c>
+    </row>
+    <row r="2152" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2152" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2152" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2152" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2152" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2152" s="2" t="s">
+        <v>2210</v>
+      </c>
+      <c r="F2152" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2152" s="4">
+        <v>-0.206040643414548</v>
+      </c>
+      <c r="H2152" s="4">
+        <v>2.0819205325399302E-2</v>
+      </c>
+      <c r="I2152" s="4">
+        <v>3.5316177670059803E-2</v>
+      </c>
+      <c r="J2152" s="4">
+        <v>1.2498742622421901E-2</v>
+      </c>
+    </row>
+    <row r="2153" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2153" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2153" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2153" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2153" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2153" s="2" t="s">
+        <v>2211</v>
+      </c>
+      <c r="F2153" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2153" s="4">
+        <v>0.36116484921158398</v>
+      </c>
+      <c r="H2153" s="4">
+        <v>2.06606376005447E-2</v>
+      </c>
+      <c r="I2153" s="6">
+        <v>-4.6010310000000002E-3</v>
+      </c>
+      <c r="J2153" s="4">
+        <v>1.3440290000000001E-2</v>
+      </c>
+    </row>
+    <row r="2154" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2154" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2154" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2154" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2154" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2154" s="2" t="s">
+        <v>2212</v>
+      </c>
+      <c r="F2154" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2154" s="4">
+        <v>0.151002873536527</v>
+      </c>
+      <c r="H2154" s="4">
+        <v>2.3051153324648899E-2</v>
+      </c>
+      <c r="I2154" s="4">
+        <v>-1.70396851924185E-2</v>
+      </c>
+      <c r="J2154" s="4">
+        <v>1.4133256043978099E-2</v>
+      </c>
+    </row>
+    <row r="2155" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2155" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2155" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2155" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2155" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2155" s="2" t="s">
+        <v>2213</v>
+      </c>
+      <c r="F2155" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2155" s="4">
+        <v>-0.24858957264568499</v>
+      </c>
+      <c r="H2155" s="4">
+        <v>3.4184478242089797E-2</v>
+      </c>
+      <c r="I2155" s="4">
+        <v>-1.504225E-2</v>
+      </c>
+      <c r="J2155" s="4">
+        <v>2.13636E-2</v>
+      </c>
+    </row>
+    <row r="2156" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2156" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2156" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2156" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2156" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2156" s="2" t="s">
+        <v>2214</v>
+      </c>
+      <c r="F2156" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2156" s="4">
+        <v>-0.25051474811034202</v>
+      </c>
+      <c r="H2156" s="4">
+        <v>3.2227267795409402E-2</v>
+      </c>
+      <c r="I2156" s="4">
+        <v>1.0227139999999999E-2</v>
+      </c>
+      <c r="J2156" s="4">
+        <v>1.9318410000000001E-2</v>
+      </c>
+    </row>
+    <row r="2157" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2157" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2157" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2157" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2157" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2157" s="2" t="s">
+        <v>2215</v>
+      </c>
+      <c r="F2157" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2157" s="4">
+        <v>0.51700648284107198</v>
+      </c>
+      <c r="H2157" s="4">
+        <v>2.4965574330464001E-2</v>
+      </c>
+      <c r="I2157" s="4">
+        <v>-9.4560789999999992E-3</v>
+      </c>
+      <c r="J2157" s="4">
+        <v>1.786749E-2</v>
+      </c>
+    </row>
+    <row r="2158" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2158" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2158" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2158" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2158" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2158" s="2" t="s">
+        <v>2216</v>
+      </c>
+      <c r="F2158" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2158" s="4">
+        <v>0.18730909830499401</v>
+      </c>
+      <c r="H2158" s="4">
+        <v>2.1236954079530801E-2</v>
+      </c>
+      <c r="I2158" s="4">
+        <v>1.7689329328908002E-2</v>
+      </c>
+      <c r="J2158" s="4">
+        <v>1.4314313632878099E-2</v>
+      </c>
+    </row>
+    <row r="2159" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2159" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2159" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2159" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2159" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2159" s="2" t="s">
+        <v>2217</v>
+      </c>
+      <c r="F2159" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2159" s="4">
+        <v>0.107957141505092</v>
+      </c>
+      <c r="H2159" s="4">
+        <v>1.8833814879594301E-2</v>
+      </c>
+      <c r="I2159" s="6">
+        <v>1.9049360000000001E-3</v>
+      </c>
+      <c r="J2159" s="4">
+        <v>1.192113E-2</v>
+      </c>
+    </row>
+    <row r="2160" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2160" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2160" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2160" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2160" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2160" s="2" t="s">
+        <v>2218</v>
+      </c>
+      <c r="F2160" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2160" s="4">
+        <v>0.16126814759612201</v>
+      </c>
+      <c r="H2160" s="4">
+        <v>2.2163242589357399E-2</v>
+      </c>
+      <c r="I2160" s="6">
+        <v>3.1899340000000002E-3</v>
+      </c>
+      <c r="J2160" s="4">
+        <v>1.472586E-2</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2161" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2161" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2161" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2161" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2161" s="2" t="s">
+        <v>2219</v>
+      </c>
+      <c r="F2161" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2161" s="4">
+        <v>0.131028262406404</v>
+      </c>
+      <c r="H2161" s="4">
+        <v>2.11511546279637E-2</v>
+      </c>
+      <c r="I2161" s="4">
+        <v>1.4344880000000001E-2</v>
+      </c>
+      <c r="J2161" s="4">
+        <v>1.3610280000000001E-2</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2162" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2162" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2162" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2162" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2162" s="2" t="s">
+        <v>2220</v>
+      </c>
+      <c r="F2162" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2162" s="4">
+        <v>1.4641808997769601</v>
+      </c>
+      <c r="H2162" s="4">
+        <v>3.8062897049766203E-2</v>
+      </c>
+      <c r="I2162" s="4">
+        <v>-1.351218E-2</v>
+      </c>
+      <c r="J2162" s="4">
+        <v>1.473678E-2</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2163" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2163" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2163" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2163" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2163" s="2" t="s">
+        <v>2221</v>
+      </c>
+      <c r="F2163" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2163" s="4">
+        <v>-0.23736925857819199</v>
+      </c>
+      <c r="H2163" s="4">
+        <v>4.1205281772274997E-2</v>
+      </c>
+      <c r="I2163" s="4">
+        <v>8.9790330000000008E-3</v>
+      </c>
+      <c r="J2163" s="4">
+        <v>2.61961E-2</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2164" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2164" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2164" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2164" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2164" s="2" t="s">
+        <v>2222</v>
+      </c>
+      <c r="F2164" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2164" s="4">
+        <v>-0.25025784380578198</v>
+      </c>
+      <c r="H2164" s="4">
+        <v>3.9210973995237403E-2</v>
+      </c>
+      <c r="I2164" s="6">
+        <v>-8.5552299999999996E-4</v>
+      </c>
+      <c r="J2164" s="4">
+        <v>2.3958030000000002E-2</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2165" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2165" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2165" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2165" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2165" s="2" t="s">
+        <v>2223</v>
+      </c>
+      <c r="F2165" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2165" s="4">
+        <v>-0.65797310555229105</v>
+      </c>
+      <c r="H2165" s="4">
+        <v>1.9804069782229899E-2</v>
+      </c>
+      <c r="I2165" s="4">
+        <v>-1.226943E-2</v>
+      </c>
+      <c r="J2165" s="4">
+        <v>1.164221E-2</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2166" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2166" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2166" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2166" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2166" s="2" t="s">
+        <v>2224</v>
+      </c>
+      <c r="F2166" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2166" s="4">
+        <v>0.72851432439723696</v>
+      </c>
+      <c r="H2166" s="4">
+        <v>2.11956717076415E-2</v>
+      </c>
+      <c r="I2166" s="4">
+        <v>5.1990430000000004E-3</v>
+      </c>
+      <c r="J2166" s="4">
+        <v>1.445081E-2</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2167" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2167" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2167" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2167" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2167" s="2" t="s">
+        <v>2225</v>
+      </c>
+      <c r="F2167" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2167" s="4">
+        <v>0.31554040058017702</v>
+      </c>
+      <c r="H2167" s="4">
+        <v>2.03653639854923E-2</v>
+      </c>
+      <c r="I2167" s="4">
+        <v>-7.3581769999999996E-3</v>
+      </c>
+      <c r="J2167" s="4">
+        <v>1.304278E-2</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2168" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2168" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2168" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2168" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2168" s="2" t="s">
+        <v>2226</v>
+      </c>
+      <c r="F2168" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2168" s="4">
+        <v>0.148420005118273</v>
+      </c>
+      <c r="H2168" s="4">
+        <v>2.21048792658156E-2</v>
+      </c>
+      <c r="I2168" s="4">
+        <v>-1.0850210000000001E-2</v>
+      </c>
+      <c r="J2168" s="4">
+        <v>1.3834050000000001E-2</v>
+      </c>
+    </row>
+    <row r="2169" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2169" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2169" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2169" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2169" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2169" s="2" t="s">
+        <v>2227</v>
+      </c>
+      <c r="F2169" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2169" s="4">
+        <v>-0.153151179494175</v>
+      </c>
+      <c r="H2169" s="4">
+        <v>2.0639941966723301E-2</v>
+      </c>
+      <c r="I2169" s="6">
+        <v>-2.8492550000000002E-3</v>
+      </c>
+      <c r="J2169" s="4">
+        <v>1.286178E-2</v>
+      </c>
+    </row>
+    <row r="2170" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2170" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2170" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2170" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2170" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2170" s="2" t="s">
+        <v>2228</v>
+      </c>
+      <c r="F2170" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2170" s="4">
+        <v>-0.116421463017251</v>
+      </c>
+      <c r="H2170" s="4">
+        <v>2.10171784107295E-2</v>
+      </c>
+      <c r="I2170" s="4">
+        <v>-5.3638030000000003E-3</v>
+      </c>
+      <c r="J2170" s="4">
+        <v>1.2839100000000001E-2</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2171" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2171" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2171" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2171" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2171" s="2" t="s">
+        <v>2229</v>
+      </c>
+      <c r="F2171" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2171" s="4">
+        <v>0.111541374732908</v>
+      </c>
+      <c r="H2171" s="4">
+        <v>1.9282970145348299E-2</v>
+      </c>
+      <c r="I2171" s="4">
+        <v>1.7519147105098502E-2</v>
+      </c>
+      <c r="J2171" s="4">
+        <v>1.2122922940646701E-2</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2172" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2172" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2172" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2172" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2172" s="2" t="s">
+        <v>2230</v>
+      </c>
+      <c r="F2172" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2172" s="4">
+        <v>-0.391414284885505</v>
+      </c>
+      <c r="H2172" s="4">
+        <v>4.2078060644459098E-2</v>
+      </c>
+      <c r="I2172" s="4">
+        <v>-1.3703142128774499E-2</v>
+      </c>
+      <c r="J2172" s="4">
+        <v>2.3483260560422499E-2</v>
+      </c>
+    </row>
+    <row r="2173" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2173" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2173" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2173" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2173" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2173" s="2" t="s">
+        <v>2231</v>
+      </c>
+      <c r="F2173" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2173" s="4">
+        <v>0.307484699747961</v>
+      </c>
+      <c r="H2173" s="4">
+        <v>2.83998818914739E-2</v>
+      </c>
+      <c r="I2173" s="4">
+        <v>2.7839302281223301E-2</v>
+      </c>
+      <c r="J2173" s="4">
+        <v>1.89503834259186E-2</v>
+      </c>
+    </row>
+    <row r="2174" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2174" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2174" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2174" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2174" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2174" s="2" t="s">
+        <v>2232</v>
+      </c>
+      <c r="F2174" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2174" s="4">
+        <v>1.0462658082959</v>
+      </c>
+      <c r="H2174" s="4">
+        <v>2.71987619521082E-2</v>
+      </c>
+      <c r="I2174" s="4">
+        <v>1.440844E-2</v>
+      </c>
+      <c r="J2174" s="4">
+        <v>2.030127E-2</v>
+      </c>
+    </row>
+    <row r="2175" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2175" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2175" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2175" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2175" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2175" s="2" t="s">
+        <v>2233</v>
+      </c>
+      <c r="F2175" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2175" s="4">
+        <v>-0.47965000629754101</v>
+      </c>
+      <c r="H2175" s="4">
+        <v>3.7483027258741003E-2</v>
+      </c>
+      <c r="I2175" s="4">
+        <v>4.15841103307696E-2</v>
+      </c>
+      <c r="J2175" s="4">
+        <v>2.5549939794983399E-2</v>
+      </c>
+    </row>
+    <row r="2176" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2176" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2176" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2176" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2176" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2176" s="2" t="s">
+        <v>2234</v>
+      </c>
+      <c r="F2176" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2176" s="4">
+        <v>0.16296882827813999</v>
+      </c>
+      <c r="H2176" s="4">
+        <v>2.9089943506996899E-2</v>
+      </c>
+      <c r="I2176" s="4">
+        <v>2.328978E-2</v>
+      </c>
+      <c r="J2176" s="4">
+        <v>1.9753369999999999E-2</v>
+      </c>
+    </row>
+    <row r="2177" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2177" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2177" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2177" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2177" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2177" s="2" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F2177" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2177" s="4">
+        <v>-0.17888746005967199</v>
+      </c>
+      <c r="H2177" s="4">
+        <v>1.88323236152577E-2</v>
+      </c>
+      <c r="I2177" s="4">
+        <v>-1.0773919999999999E-2</v>
+      </c>
+      <c r="J2177" s="4">
+        <v>1.188435E-2</v>
+      </c>
+    </row>
+    <row r="2178" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2178" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2178" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2178" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2178" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2178" s="2" t="s">
+        <v>2236</v>
+      </c>
+      <c r="F2178" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2178" s="4">
+        <v>-0.30029461050262501</v>
+      </c>
+      <c r="H2178" s="4">
+        <v>3.9403522889186499E-2</v>
+      </c>
+      <c r="I2178" s="6">
+        <v>3.085029E-3</v>
+      </c>
+      <c r="J2178" s="4">
+        <v>2.606822E-2</v>
+      </c>
+    </row>
+    <row r="2179" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2179" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2179" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2179" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2179" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2179" s="2" t="s">
+        <v>2237</v>
+      </c>
+      <c r="F2179" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2179" s="4">
+        <v>-0.79407309914990598</v>
+      </c>
+      <c r="H2179" s="4">
+        <v>2.1290572476686299E-2</v>
+      </c>
+      <c r="I2179" s="6">
+        <v>-2.101384E-3</v>
+      </c>
+      <c r="J2179" s="4">
+        <v>1.1882159999999999E-2</v>
+      </c>
+    </row>
+    <row r="2180" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2180" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2180" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2180" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2180" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2180" s="2" t="s">
+        <v>2238</v>
+      </c>
+      <c r="F2180" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2180" s="4">
+        <v>-0.80251571761531004</v>
+      </c>
+      <c r="H2180" s="4">
+        <v>2.1452690710366599E-2</v>
+      </c>
+      <c r="I2180" s="4">
+        <v>-1.0011890000000001E-2</v>
+      </c>
+      <c r="J2180" s="4">
+        <v>1.190038E-2</v>
+      </c>
+    </row>
+    <row r="2181" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2181" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2181" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2181" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2181" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2181" s="2" t="s">
+        <v>2239</v>
+      </c>
+      <c r="F2181" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2181" s="4">
+        <v>1.55371376366174</v>
+      </c>
+      <c r="H2181" s="4">
+        <v>4.0390396459938901E-2</v>
+      </c>
+      <c r="I2181" s="4">
+        <v>-5.7061430000000003E-3</v>
+      </c>
+      <c r="J2181" s="4">
+        <v>1.429533E-2</v>
+      </c>
+    </row>
+    <row r="2182" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2182" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2182" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2182" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2182" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2182" s="2" t="s">
+        <v>2240</v>
+      </c>
+      <c r="F2182" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2182" s="4">
+        <v>-1.35634728475194</v>
+      </c>
+      <c r="H2182" s="4">
+        <v>3.5259650683263997E-2</v>
+      </c>
+      <c r="I2182" s="4">
+        <v>3.1299579809244797E-2</v>
+      </c>
+      <c r="J2182" s="4">
+        <v>1.1731402482274301E-2</v>
+      </c>
+    </row>
+    <row r="2183" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2183" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2183" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2183" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2183" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2183" s="2" t="s">
+        <v>2241</v>
+      </c>
+      <c r="F2183" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2183" s="4">
+        <v>0.83421262083854797</v>
+      </c>
+      <c r="H2183" s="4">
+        <v>3.1817306243431001E-2</v>
+      </c>
+      <c r="I2183" s="4">
+        <v>1.542381E-2</v>
+      </c>
+      <c r="J2183" s="4">
+        <v>2.43815E-2</v>
+      </c>
+    </row>
+    <row r="2184" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A2184" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2184" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2184" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2184" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2184" s="2" t="s">
+        <v>2242</v>
+      </c>
+      <c r="F2184" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2184" s="4">
+        <v>-0.36614824573121402</v>
+      </c>
+      <c r="H2184" s="4">
+        <v>4.4957988910013798E-2</v>
+      </c>
+      <c r="I2184" s="4">
+        <v>-3.9001412108437897E-2</v>
+      </c>
+      <c r="J2184" s="4">
+        <v>2.9645221535035599E-2</v>
+      </c>
+    </row>
+    <row r="2185" spans="1:10" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2185" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B2185" t="s">
+        <v>2136</v>
+      </c>
+      <c r="C2185" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D2185" t="s">
+        <v>2138</v>
+      </c>
+      <c r="E2185" s="3" t="s">
+        <v>2243</v>
+      </c>
+      <c r="F2185" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2185" s="5">
+        <v>0.17814618538347399</v>
+      </c>
+      <c r="H2185" s="5">
+        <v>2.15135389150726E-2</v>
+      </c>
+      <c r="I2185" s="7">
+        <v>1.1593370000000001E-3</v>
+      </c>
+      <c r="J2185" s="5">
+        <v>1.3474160000000001E-2</v>
+      </c>
+    </row>
+    <row r="2186" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
+      <c r="A2186" t="s">
+        <v>2244</v>
+      </c>
+      <c r="B2186" t="s">
+        <v>2245</v>
+      </c>
+      <c r="C2186" t="s">
+        <v>1487</v>
+      </c>
+      <c r="D2186" t="s">
+        <v>2246</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>